<commit_message>
chore(files): Add all countries to excel format
</commit_message>
<xml_diff>
--- a/Psytech/public/excel/Formato_Importar_Aspirantes.xlsx
+++ b/Psytech/public/excel/Formato_Importar_Aspirantes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecmx-my.sharepoint.com/personal/a01712218_tec_mx/Documents/Desktop/Semestre 4/VaultTech/VaultTech-Nombre-del-Proyecto-/Psytech/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\OneDrive - Instituto Tecnologico y de Estudios Superiores de Monterrey\Desktop\Semestre 4\VaultTech\VaultTech-Nombre-del-Proyecto-\Psytech\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{8303559A-5284-420E-88BE-465117EC11D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F9DC3AB-B7E1-4796-B02D-51B10CBAD7EA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52EB75A-E6EC-4EEC-A791-A5D7BBC9BED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="59040" yWindow="-4065" windowWidth="17280" windowHeight="8880" xr2:uid="{9EF69BDA-D6A3-4D3E-875F-AFA57B479CB3}"/>
+    <workbookView xWindow="28680" yWindow="-5535" windowWidth="29040" windowHeight="15720" xr2:uid="{9EF69BDA-D6A3-4D3E-875F-AFA57B479CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Aspirantes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="235">
   <si>
     <t>Paises</t>
   </si>
@@ -82,13 +82,673 @@
   </si>
   <si>
     <t>Jalisco</t>
+  </si>
+  <si>
+    <t>Afganistán</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Alemania</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Antigua y Barbuda</t>
+  </si>
+  <si>
+    <t>Arabia Saudita</t>
+  </si>
+  <si>
+    <t>Argelia</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Azerbaiyán</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Bangladés</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Baréin</t>
+  </si>
+  <si>
+    <t>Bélgica</t>
+  </si>
+  <si>
+    <t>Belice</t>
+  </si>
+  <si>
+    <t>Benín</t>
+  </si>
+  <si>
+    <t>Bielorrusia</t>
+  </si>
+  <si>
+    <t>Birmania</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Bosnia y Herzegovina</t>
+  </si>
+  <si>
+    <t>Botsuana</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>Brunéi</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Bután</t>
+  </si>
+  <si>
+    <t>Cabo Verde</t>
+  </si>
+  <si>
+    <t>Camboya</t>
+  </si>
+  <si>
+    <t>Camerún</t>
+  </si>
+  <si>
+    <t>Canadá</t>
+  </si>
+  <si>
+    <t>Catar</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Chipre</t>
+  </si>
+  <si>
+    <t>Ciudad del Vaticano</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Comoras</t>
+  </si>
+  <si>
+    <t>Corea del Norte</t>
+  </si>
+  <si>
+    <t>Corea del Sur</t>
+  </si>
+  <si>
+    <t>Costa de Marfil</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Dinamarca</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Egipto</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Emiratos Árabes Unidos</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Eslovaquia</t>
+  </si>
+  <si>
+    <t>Eslovenia</t>
+  </si>
+  <si>
+    <t>España</t>
+  </si>
+  <si>
+    <t>Estados Unidos</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Etiopía</t>
+  </si>
+  <si>
+    <t>Filipinas</t>
+  </si>
+  <si>
+    <t>Finlandia</t>
+  </si>
+  <si>
+    <t>Fiyi</t>
+  </si>
+  <si>
+    <t>Francia</t>
+  </si>
+  <si>
+    <t>Gabón</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Granada</t>
+  </si>
+  <si>
+    <t>Grecia</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Guinea ecuatorial</t>
+  </si>
+  <si>
+    <t>Guinea-Bisáu</t>
+  </si>
+  <si>
+    <t>Haití</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Hungría</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Irak</t>
+  </si>
+  <si>
+    <t>Irán</t>
+  </si>
+  <si>
+    <t>Irlanda</t>
+  </si>
+  <si>
+    <t>Islandia</t>
+  </si>
+  <si>
+    <t>Islas Marshall</t>
+  </si>
+  <si>
+    <t>Islas Salomón</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Japón</t>
+  </si>
+  <si>
+    <t>Jordania</t>
+  </si>
+  <si>
+    <t>Kazajistán</t>
+  </si>
+  <si>
+    <t>Kenia</t>
+  </si>
+  <si>
+    <t>Kirguistán</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Lesoto</t>
+  </si>
+  <si>
+    <t>Letonia</t>
+  </si>
+  <si>
+    <t>Líbano</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Libia</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Lituania</t>
+  </si>
+  <si>
+    <t>Luxemburgo</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Malasia</t>
+  </si>
+  <si>
+    <t>Malaui</t>
+  </si>
+  <si>
+    <t>Maldivas</t>
+  </si>
+  <si>
+    <t>Malí</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Marruecos</t>
+  </si>
+  <si>
+    <t>Mauricio</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Micronesia</t>
+  </si>
+  <si>
+    <t>Moldavia</t>
+  </si>
+  <si>
+    <t>Mónaco</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Níger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Noruega</t>
+  </si>
+  <si>
+    <t>Nueva Zelanda</t>
+  </si>
+  <si>
+    <t>Omán</t>
+  </si>
+  <si>
+    <t>Países Bajos</t>
+  </si>
+  <si>
+    <t>Pakistán</t>
+  </si>
+  <si>
+    <t>Palaos</t>
+  </si>
+  <si>
+    <t>Panamá</t>
+  </si>
+  <si>
+    <t>Papúa Nueva Guinea</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Perú</t>
+  </si>
+  <si>
+    <t>Polonia</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Reino Unido</t>
+  </si>
+  <si>
+    <t>República Centroafricana</t>
+  </si>
+  <si>
+    <t>República Checa</t>
+  </si>
+  <si>
+    <t>República de Macedonia</t>
+  </si>
+  <si>
+    <t>República del Congo</t>
+  </si>
+  <si>
+    <t>República Democrática del Congo</t>
+  </si>
+  <si>
+    <t>República Dominicana</t>
+  </si>
+  <si>
+    <t>República Sudafricana</t>
+  </si>
+  <si>
+    <t>Ruanda</t>
+  </si>
+  <si>
+    <t>Rumanía</t>
+  </si>
+  <si>
+    <t>Rusia</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>San Cristóbal y Nieves</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>San Vicente y las Granadinas</t>
+  </si>
+  <si>
+    <t>Santa Lucía</t>
+  </si>
+  <si>
+    <t>Santo Tomé y Príncipe</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Sierra Leona</t>
+  </si>
+  <si>
+    <t>Singapur</t>
+  </si>
+  <si>
+    <t>Siria</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Suazilandia</t>
+  </si>
+  <si>
+    <t>Sudáfrica</t>
+  </si>
+  <si>
+    <t>Sudán</t>
+  </si>
+  <si>
+    <t>Sudán del Sur</t>
+  </si>
+  <si>
+    <t>Suecia</t>
+  </si>
+  <si>
+    <t>Suiza</t>
+  </si>
+  <si>
+    <t>Surinam</t>
+  </si>
+  <si>
+    <t>Tailandia</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Tayikistán</t>
+  </si>
+  <si>
+    <t>Timor Oriental</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Trinidad y Tobago</t>
+  </si>
+  <si>
+    <t>Túnez</t>
+  </si>
+  <si>
+    <t>Turkmenistán</t>
+  </si>
+  <si>
+    <t>Turquía</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>Ucrania</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Uzbekistán</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Yibuti</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabue</t>
+  </si>
+  <si>
+    <t>Aguascalientes</t>
+  </si>
+  <si>
+    <t>Baja California</t>
+  </si>
+  <si>
+    <t>Baja California Sur</t>
+  </si>
+  <si>
+    <t>Campeche</t>
+  </si>
+  <si>
+    <t>Chiapas</t>
+  </si>
+  <si>
+    <t>Chihuahua</t>
+  </si>
+  <si>
+    <t>Coahuila</t>
+  </si>
+  <si>
+    <t>Colima</t>
+  </si>
+  <si>
+    <t>Durango</t>
+  </si>
+  <si>
+    <t>Guanajuato</t>
+  </si>
+  <si>
+    <t>Guerrero</t>
+  </si>
+  <si>
+    <t>Hidalgo</t>
+  </si>
+  <si>
+    <t>Estado de México</t>
+  </si>
+  <si>
+    <t>Michoacán</t>
+  </si>
+  <si>
+    <t>Morelos</t>
+  </si>
+  <si>
+    <t>Nayarit</t>
+  </si>
+  <si>
+    <t>Nuevo León</t>
+  </si>
+  <si>
+    <t>Oaxaca</t>
+  </si>
+  <si>
+    <t>Puebla</t>
+  </si>
+  <si>
+    <t>Quintana Roo</t>
+  </si>
+  <si>
+    <t>San Luis Potosí</t>
+  </si>
+  <si>
+    <t>Sinaloa</t>
+  </si>
+  <si>
+    <t>Sonora</t>
+  </si>
+  <si>
+    <t>Tabasco</t>
+  </si>
+  <si>
+    <t>Tamaulipas</t>
+  </si>
+  <si>
+    <t>Tlaxcala</t>
+  </si>
+  <si>
+    <t>Veracruz</t>
+  </si>
+  <si>
+    <t>Yucatán</t>
+  </si>
+  <si>
+    <t>Zacatecas</t>
+  </si>
+  <si>
+    <t>Ciudad de México</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +759,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,11 +825,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +1175,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E00EE5-E118-4BFC-8E55-3A0C9A42EE68}">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2780,36 +3451,1080 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0424DF52-A05E-469F-9FCA-0757AA06F133}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>